<commit_message>
Now sorting by distributor for easy ordering
</commit_message>
<xml_diff>
--- a/BOM-MASTER.xlsx
+++ b/BOM-MASTER.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jrye/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jrye/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -2104,8 +2104,8 @@
   <dimension ref="A1:AB990"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A120" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C150" sqref="C150"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2176,8 +2176,8 @@
       <c r="D2" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="9" t="s">
-        <v>10</v>
+      <c r="E2" s="33" t="s">
+        <v>454</v>
       </c>
       <c r="F2" s="12"/>
       <c r="G2" s="9"/>
@@ -2217,7 +2217,7 @@
         <v>14</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>15</v>
+        <v>74</v>
       </c>
       <c r="F3" s="12"/>
       <c r="G3" s="17" t="s">
@@ -2259,7 +2259,7 @@
         <v>43</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>15</v>
+        <v>74</v>
       </c>
       <c r="F4" s="12"/>
       <c r="G4" s="17" t="s">
@@ -2300,7 +2300,7 @@
       <c r="D5" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E5" s="33" t="s">
         <v>74</v>
       </c>
       <c r="F5" s="20"/>
@@ -2381,7 +2381,7 @@
         <v>91</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>18</v>
+        <v>74</v>
       </c>
       <c r="F7" s="15" t="s">
         <v>94</v>
@@ -2423,7 +2423,7 @@
         <v>104</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>107</v>
+        <v>74</v>
       </c>
       <c r="F8" s="12"/>
       <c r="G8" s="9"/>
@@ -2463,7 +2463,7 @@
         <v>114</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>122</v>
+        <v>74</v>
       </c>
       <c r="F9" s="12"/>
       <c r="G9" s="9"/>
@@ -2503,7 +2503,7 @@
         <v>114</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>122</v>
+        <v>74</v>
       </c>
       <c r="F10" s="12"/>
       <c r="G10" s="9"/>
@@ -2543,7 +2543,7 @@
         <v>114</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>122</v>
+        <v>74</v>
       </c>
       <c r="F11" s="12"/>
       <c r="G11" s="9"/>
@@ -2582,7 +2582,7 @@
       <c r="D12" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="E12" s="12" t="s">
+      <c r="E12" s="17" t="s">
         <v>74</v>
       </c>
       <c r="F12" s="12"/>
@@ -2622,8 +2622,8 @@
       <c r="D13" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="E13" s="12" t="s">
-        <v>155</v>
+      <c r="E13" s="17" t="s">
+        <v>74</v>
       </c>
       <c r="F13" s="12"/>
       <c r="G13" s="9"/>
@@ -2904,7 +2904,7 @@
       <c r="D20" s="10" t="s">
         <v>202</v>
       </c>
-      <c r="E20" s="9" t="s">
+      <c r="E20" s="33" t="s">
         <v>74</v>
       </c>
       <c r="F20" s="12"/>
@@ -2944,7 +2944,7 @@
       <c r="D21" s="10" t="s">
         <v>206</v>
       </c>
-      <c r="E21" s="9" t="s">
+      <c r="E21" s="33" t="s">
         <v>74</v>
       </c>
       <c r="F21" s="12"/>
@@ -2984,7 +2984,7 @@
       <c r="D22" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="E22" s="9" t="s">
+      <c r="E22" s="33" t="s">
         <v>74</v>
       </c>
       <c r="F22" s="12"/>
@@ -3024,7 +3024,7 @@
       <c r="D23" s="10" t="s">
         <v>215</v>
       </c>
-      <c r="E23" s="9" t="s">
+      <c r="E23" s="33" t="s">
         <v>74</v>
       </c>
       <c r="F23" s="12"/>
@@ -3064,7 +3064,7 @@
       <c r="D24" s="10" t="s">
         <v>220</v>
       </c>
-      <c r="E24" s="9" t="s">
+      <c r="E24" s="33" t="s">
         <v>74</v>
       </c>
       <c r="F24" s="12"/>
@@ -3225,7 +3225,7 @@
         <v>230</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>15</v>
+        <v>74</v>
       </c>
       <c r="F28" s="12"/>
       <c r="G28" s="9"/>
@@ -3304,8 +3304,8 @@
       <c r="D30" s="22" t="s">
         <v>236</v>
       </c>
-      <c r="E30" s="17" t="s">
-        <v>239</v>
+      <c r="E30" s="33" t="s">
+        <v>74</v>
       </c>
       <c r="F30" s="12"/>
       <c r="G30" s="9"/>
@@ -3345,7 +3345,7 @@
         <v>240</v>
       </c>
       <c r="E31" s="12" t="s">
-        <v>15</v>
+        <v>74</v>
       </c>
       <c r="F31" s="12"/>
       <c r="G31" s="9"/>
@@ -3545,7 +3545,7 @@
         <v>255</v>
       </c>
       <c r="E36" s="12" t="s">
-        <v>15</v>
+        <v>74</v>
       </c>
       <c r="F36" s="12"/>
       <c r="G36" s="9"/>
@@ -3584,8 +3584,8 @@
       <c r="D37" s="10" t="s">
         <v>256</v>
       </c>
-      <c r="E37" s="12" t="s">
-        <v>15</v>
+      <c r="E37" s="17" t="s">
+        <v>275</v>
       </c>
       <c r="F37" s="12"/>
       <c r="G37" s="9"/>
@@ -3625,7 +3625,7 @@
         <v>262</v>
       </c>
       <c r="E38" s="9" t="s">
-        <v>15</v>
+        <v>275</v>
       </c>
       <c r="F38" s="12"/>
       <c r="G38" s="9"/>
@@ -3665,7 +3665,7 @@
         <v>265</v>
       </c>
       <c r="E39" s="9" t="s">
-        <v>15</v>
+        <v>275</v>
       </c>
       <c r="F39" s="12"/>
       <c r="G39" s="9"/>
@@ -3705,7 +3705,7 @@
         <v>268</v>
       </c>
       <c r="E40" s="9" t="s">
-        <v>74</v>
+        <v>275</v>
       </c>
       <c r="F40" s="12"/>
       <c r="G40" s="9"/>
@@ -3744,8 +3744,8 @@
       <c r="D41" s="10" t="s">
         <v>270</v>
       </c>
-      <c r="E41" s="12" t="s">
-        <v>271</v>
+      <c r="E41" s="17" t="s">
+        <v>275</v>
       </c>
       <c r="F41" s="12"/>
       <c r="G41" s="9"/>
@@ -3785,7 +3785,7 @@
         <v>273</v>
       </c>
       <c r="E42" s="9" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="F42" s="12"/>
       <c r="G42" s="9"/>
@@ -3904,8 +3904,8 @@
       <c r="D45" s="10" t="s">
         <v>277</v>
       </c>
-      <c r="E45" s="9" t="s">
-        <v>278</v>
+      <c r="E45" s="33" t="s">
+        <v>148</v>
       </c>
       <c r="F45" s="12"/>
       <c r="G45" s="9"/>
@@ -3944,8 +3944,8 @@
       <c r="D46" s="10" t="s">
         <v>279</v>
       </c>
-      <c r="E46" s="9" t="s">
-        <v>275</v>
+      <c r="E46" s="33" t="s">
+        <v>500</v>
       </c>
       <c r="F46" s="12"/>
       <c r="G46" s="9"/>
@@ -3985,7 +3985,7 @@
         <v>282</v>
       </c>
       <c r="E47" s="9" t="s">
-        <v>74</v>
+        <v>239</v>
       </c>
       <c r="F47" s="12"/>
       <c r="G47" s="9" t="s">
@@ -4026,8 +4026,8 @@
       <c r="D48" s="10" t="s">
         <v>288</v>
       </c>
-      <c r="E48" s="9" t="s">
-        <v>275</v>
+      <c r="E48" s="33" t="s">
+        <v>430</v>
       </c>
       <c r="F48" s="12"/>
       <c r="G48" s="9"/>
@@ -4066,8 +4066,8 @@
       <c r="D49" s="10" t="s">
         <v>294</v>
       </c>
-      <c r="E49" s="9" t="s">
-        <v>74</v>
+      <c r="E49" s="33" t="s">
+        <v>430</v>
       </c>
       <c r="F49" s="12"/>
       <c r="G49" s="9"/>
@@ -4107,7 +4107,7 @@
         <v>299</v>
       </c>
       <c r="E50" s="12" t="s">
-        <v>10</v>
+        <v>430</v>
       </c>
       <c r="F50" s="12"/>
       <c r="G50" s="9"/>
@@ -4147,7 +4147,7 @@
         <v>306</v>
       </c>
       <c r="E51" s="12" t="s">
-        <v>307</v>
+        <v>430</v>
       </c>
       <c r="F51" s="12"/>
       <c r="G51" s="9"/>
@@ -4187,7 +4187,7 @@
         <v>310</v>
       </c>
       <c r="E52" s="9" t="s">
-        <v>275</v>
+        <v>15</v>
       </c>
       <c r="F52" s="12"/>
       <c r="G52" s="9"/>
@@ -4227,7 +4227,7 @@
         <v>313</v>
       </c>
       <c r="E53" s="9" t="s">
-        <v>275</v>
+        <v>15</v>
       </c>
       <c r="F53" s="12"/>
       <c r="G53" s="9"/>
@@ -4266,8 +4266,8 @@
       <c r="D54" s="10" t="s">
         <v>316</v>
       </c>
-      <c r="E54" s="9" t="s">
-        <v>275</v>
+      <c r="E54" s="33" t="s">
+        <v>15</v>
       </c>
       <c r="F54" s="12"/>
       <c r="G54" s="9"/>
@@ -4306,8 +4306,8 @@
       <c r="D55" s="10" t="s">
         <v>319</v>
       </c>
-      <c r="E55" s="9" t="s">
-        <v>275</v>
+      <c r="E55" s="33" t="s">
+        <v>15</v>
       </c>
       <c r="F55" s="12"/>
       <c r="G55" s="9"/>
@@ -4346,8 +4346,8 @@
       <c r="D56" s="10" t="s">
         <v>320</v>
       </c>
-      <c r="E56" s="9" t="s">
-        <v>259</v>
+      <c r="E56" s="33" t="s">
+        <v>15</v>
       </c>
       <c r="F56" s="12" t="s">
         <v>321</v>
@@ -4388,8 +4388,8 @@
       <c r="D57" s="10" t="s">
         <v>322</v>
       </c>
-      <c r="E57" s="9" t="s">
-        <v>259</v>
+      <c r="E57" s="33" t="s">
+        <v>15</v>
       </c>
       <c r="F57" s="12" t="s">
         <v>323</v>
@@ -4431,7 +4431,7 @@
         <v>324</v>
       </c>
       <c r="E58" s="9" t="s">
-        <v>259</v>
+        <v>15</v>
       </c>
       <c r="F58" s="12" t="s">
         <v>325</v>
@@ -4472,8 +4472,8 @@
       <c r="D59" s="10" t="s">
         <v>326</v>
       </c>
-      <c r="E59" s="15" t="s">
-        <v>286</v>
+      <c r="E59" s="17" t="s">
+        <v>15</v>
       </c>
       <c r="F59" s="11"/>
       <c r="G59" s="17"/>
@@ -4513,7 +4513,7 @@
         <v>327</v>
       </c>
       <c r="E60" s="15" t="s">
-        <v>328</v>
+        <v>15</v>
       </c>
       <c r="F60" s="11"/>
       <c r="G60" s="17"/>
@@ -4553,7 +4553,7 @@
         <v>329</v>
       </c>
       <c r="E61" s="15" t="s">
-        <v>74</v>
+        <v>15</v>
       </c>
       <c r="F61" s="11"/>
       <c r="G61" s="17"/>
@@ -4592,8 +4592,8 @@
       <c r="D62" s="31" t="s">
         <v>330</v>
       </c>
-      <c r="E62" s="16" t="s">
-        <v>331</v>
+      <c r="E62" s="33" t="s">
+        <v>15</v>
       </c>
       <c r="F62" s="15"/>
       <c r="G62" s="17"/>
@@ -4632,8 +4632,8 @@
       <c r="D63" s="31" t="s">
         <v>332</v>
       </c>
-      <c r="E63" s="16" t="s">
-        <v>331</v>
+      <c r="E63" s="33" t="s">
+        <v>15</v>
       </c>
       <c r="F63" s="15" t="s">
         <v>333</v>
@@ -4675,7 +4675,7 @@
         <v>336</v>
       </c>
       <c r="E64" s="15" t="s">
-        <v>337</v>
+        <v>15</v>
       </c>
       <c r="F64" s="12" t="s">
         <v>338</v>
@@ -4717,7 +4717,7 @@
         <v>336</v>
       </c>
       <c r="E65" s="15" t="s">
-        <v>337</v>
+        <v>15</v>
       </c>
       <c r="F65" s="12" t="s">
         <v>341</v>
@@ -4759,7 +4759,7 @@
         <v>336</v>
       </c>
       <c r="E66" s="15" t="s">
-        <v>337</v>
+        <v>15</v>
       </c>
       <c r="F66" s="12" t="s">
         <v>344</v>
@@ -4801,7 +4801,7 @@
         <v>336</v>
       </c>
       <c r="E67" s="15" t="s">
-        <v>337</v>
+        <v>15</v>
       </c>
       <c r="F67" s="12" t="s">
         <v>347</v>
@@ -4923,7 +4923,7 @@
         <v>336</v>
       </c>
       <c r="E70" s="15" t="s">
-        <v>337</v>
+        <v>15</v>
       </c>
       <c r="F70" s="12" t="s">
         <v>356</v>
@@ -4965,7 +4965,7 @@
         <v>336</v>
       </c>
       <c r="E71" s="15" t="s">
-        <v>337</v>
+        <v>15</v>
       </c>
       <c r="F71" s="12" t="s">
         <v>359</v>
@@ -5007,7 +5007,7 @@
         <v>336</v>
       </c>
       <c r="E72" s="15" t="s">
-        <v>337</v>
+        <v>15</v>
       </c>
       <c r="F72" s="12" t="s">
         <v>362</v>
@@ -5091,7 +5091,7 @@
         <v>367</v>
       </c>
       <c r="E74" s="12" t="s">
-        <v>74</v>
+        <v>15</v>
       </c>
       <c r="F74" s="12"/>
       <c r="G74" s="9"/>
@@ -5131,7 +5131,7 @@
         <v>368</v>
       </c>
       <c r="E75" s="15" t="s">
-        <v>74</v>
+        <v>15</v>
       </c>
       <c r="F75" s="11"/>
       <c r="G75" s="17"/>
@@ -5171,7 +5171,7 @@
         <v>336</v>
       </c>
       <c r="E76" s="12" t="s">
-        <v>337</v>
+        <v>15</v>
       </c>
       <c r="F76" s="12" t="s">
         <v>371</v>
@@ -5212,8 +5212,8 @@
       <c r="D77" s="32" t="s">
         <v>374</v>
       </c>
-      <c r="E77" s="33" t="s">
-        <v>15</v>
+      <c r="E77" s="17" t="s">
+        <v>259</v>
       </c>
       <c r="F77" s="12"/>
       <c r="G77" s="9"/>
@@ -5252,8 +5252,8 @@
       <c r="D78" s="32" t="s">
         <v>377</v>
       </c>
-      <c r="E78" s="33" t="s">
-        <v>15</v>
+      <c r="E78" s="17" t="s">
+        <v>259</v>
       </c>
       <c r="F78" s="12"/>
       <c r="G78" s="9"/>
@@ -5292,8 +5292,8 @@
       <c r="D79" s="32" t="s">
         <v>380</v>
       </c>
-      <c r="E79" s="33" t="s">
-        <v>15</v>
+      <c r="E79" s="17" t="s">
+        <v>259</v>
       </c>
       <c r="F79" s="12"/>
       <c r="G79" s="9"/>
@@ -5333,7 +5333,7 @@
         <v>383</v>
       </c>
       <c r="E80" s="33" t="s">
-        <v>15</v>
+        <v>259</v>
       </c>
       <c r="F80" s="12"/>
       <c r="G80" s="9"/>
@@ -5372,8 +5372,8 @@
       <c r="D81" s="32" t="s">
         <v>386</v>
       </c>
-      <c r="E81" s="33" t="s">
-        <v>15</v>
+      <c r="E81" s="17" t="s">
+        <v>122</v>
       </c>
       <c r="F81" s="12"/>
       <c r="G81" s="9"/>
@@ -5412,8 +5412,8 @@
       <c r="D82" s="32" t="s">
         <v>389</v>
       </c>
-      <c r="E82" s="33" t="s">
-        <v>15</v>
+      <c r="E82" s="17" t="s">
+        <v>122</v>
       </c>
       <c r="F82" s="12"/>
       <c r="G82" s="9"/>
@@ -5452,8 +5452,8 @@
       <c r="D83" s="32" t="s">
         <v>392</v>
       </c>
-      <c r="E83" s="33" t="s">
-        <v>15</v>
+      <c r="E83" s="17" t="s">
+        <v>122</v>
       </c>
       <c r="F83" s="12"/>
       <c r="G83" s="9"/>
@@ -5493,7 +5493,7 @@
         <v>395</v>
       </c>
       <c r="E84" s="33" t="s">
-        <v>15</v>
+        <v>448</v>
       </c>
       <c r="F84" s="12"/>
       <c r="G84" s="9"/>
@@ -5532,8 +5532,8 @@
       <c r="D85" s="32" t="s">
         <v>398</v>
       </c>
-      <c r="E85" s="33" t="s">
-        <v>15</v>
+      <c r="E85" s="17" t="s">
+        <v>18</v>
       </c>
       <c r="F85" s="12"/>
       <c r="G85" s="9"/>
@@ -5572,8 +5572,8 @@
       <c r="D86" s="32" t="s">
         <v>401</v>
       </c>
-      <c r="E86" s="33" t="s">
-        <v>15</v>
+      <c r="E86" s="17" t="s">
+        <v>331</v>
       </c>
       <c r="F86" s="12"/>
       <c r="G86" s="9"/>
@@ -5612,8 +5612,8 @@
       <c r="D87" s="32" t="s">
         <v>404</v>
       </c>
-      <c r="E87" s="15" t="s">
-        <v>15</v>
+      <c r="E87" s="17" t="s">
+        <v>331</v>
       </c>
       <c r="F87" s="12"/>
       <c r="G87" s="9"/>
@@ -5653,7 +5653,7 @@
         <v>407</v>
       </c>
       <c r="E88" s="33" t="s">
-        <v>15</v>
+        <v>331</v>
       </c>
       <c r="F88" s="12"/>
       <c r="G88" s="9"/>
@@ -5693,7 +5693,7 @@
         <v>410</v>
       </c>
       <c r="E89" s="33" t="s">
-        <v>15</v>
+        <v>331</v>
       </c>
       <c r="F89" s="12"/>
       <c r="G89" s="9"/>
@@ -5733,7 +5733,7 @@
         <v>413</v>
       </c>
       <c r="E90" s="33" t="s">
-        <v>15</v>
+        <v>331</v>
       </c>
       <c r="F90" s="12"/>
       <c r="G90" s="9"/>
@@ -5773,7 +5773,7 @@
         <v>416</v>
       </c>
       <c r="E91" s="12" t="s">
-        <v>74</v>
+        <v>331</v>
       </c>
       <c r="F91" s="12"/>
       <c r="G91" s="9"/>
@@ -5813,7 +5813,7 @@
         <v>419</v>
       </c>
       <c r="E92" s="33" t="s">
-        <v>74</v>
+        <v>331</v>
       </c>
       <c r="F92" s="12"/>
       <c r="G92" s="9"/>
@@ -5853,7 +5853,7 @@
         <v>422</v>
       </c>
       <c r="E93" s="12" t="s">
-        <v>74</v>
+        <v>331</v>
       </c>
       <c r="F93" s="12"/>
       <c r="G93" s="9"/>
@@ -5893,7 +5893,7 @@
         <v>425</v>
       </c>
       <c r="E94" s="33" t="s">
-        <v>259</v>
+        <v>331</v>
       </c>
       <c r="F94" s="11" t="s">
         <v>426</v>
@@ -5935,7 +5935,7 @@
         <v>429</v>
       </c>
       <c r="E95" s="33" t="s">
-        <v>430</v>
+        <v>331</v>
       </c>
       <c r="F95" s="11"/>
       <c r="G95" s="9"/>
@@ -5975,7 +5975,7 @@
         <v>433</v>
       </c>
       <c r="E96" s="33" t="s">
-        <v>430</v>
+        <v>331</v>
       </c>
       <c r="F96" s="11"/>
       <c r="G96" s="9"/>
@@ -6015,7 +6015,7 @@
         <v>436</v>
       </c>
       <c r="E97" s="33" t="s">
-        <v>430</v>
+        <v>331</v>
       </c>
       <c r="F97" s="11"/>
       <c r="G97" s="9"/>
@@ -6055,7 +6055,7 @@
         <v>436</v>
       </c>
       <c r="E98" s="33" t="s">
-        <v>430</v>
+        <v>331</v>
       </c>
       <c r="F98" s="11"/>
       <c r="G98" s="9"/>
@@ -6135,7 +6135,7 @@
         <v>444</v>
       </c>
       <c r="E100" s="33" t="s">
-        <v>74</v>
+        <v>331</v>
       </c>
       <c r="F100" s="11"/>
       <c r="G100" s="9"/>
@@ -6175,7 +6175,7 @@
         <v>447</v>
       </c>
       <c r="E101" s="33" t="s">
-        <v>448</v>
+        <v>331</v>
       </c>
       <c r="F101" s="11"/>
       <c r="G101" s="9"/>
@@ -6253,7 +6253,7 @@
         <v>114</v>
       </c>
       <c r="E103" s="33" t="s">
-        <v>454</v>
+        <v>331</v>
       </c>
       <c r="F103" s="11"/>
       <c r="G103" s="9"/>
@@ -6293,7 +6293,7 @@
         <v>457</v>
       </c>
       <c r="E104" s="33" t="s">
-        <v>458</v>
+        <v>331</v>
       </c>
       <c r="F104" s="11"/>
       <c r="G104" s="9"/>
@@ -6333,7 +6333,7 @@
         <v>457</v>
       </c>
       <c r="E105" s="33" t="s">
-        <v>458</v>
+        <v>331</v>
       </c>
       <c r="F105" s="11"/>
       <c r="G105" s="9"/>
@@ -6373,7 +6373,7 @@
         <v>463</v>
       </c>
       <c r="E106" s="33" t="s">
-        <v>74</v>
+        <v>331</v>
       </c>
       <c r="F106" s="11"/>
       <c r="G106" s="9"/>
@@ -6413,7 +6413,7 @@
         <v>466</v>
       </c>
       <c r="E107" s="33" t="s">
-        <v>74</v>
+        <v>331</v>
       </c>
       <c r="F107" s="11"/>
       <c r="G107" s="9"/>
@@ -7251,7 +7251,7 @@
         <v>486</v>
       </c>
       <c r="E127" s="33" t="s">
-        <v>331</v>
+        <v>155</v>
       </c>
       <c r="F127" s="11" t="s">
         <v>95</v>
@@ -7293,7 +7293,7 @@
         <v>487</v>
       </c>
       <c r="E128" s="33" t="s">
-        <v>331</v>
+        <v>307</v>
       </c>
       <c r="F128" s="11" t="s">
         <v>100</v>
@@ -7335,7 +7335,7 @@
         <v>488</v>
       </c>
       <c r="E129" s="33" t="s">
-        <v>331</v>
+        <v>337</v>
       </c>
       <c r="F129" s="11" t="s">
         <v>103</v>
@@ -7377,7 +7377,7 @@
         <v>489</v>
       </c>
       <c r="E130" s="33" t="s">
-        <v>331</v>
+        <v>337</v>
       </c>
       <c r="F130" s="11" t="s">
         <v>108</v>
@@ -7419,7 +7419,7 @@
         <v>490</v>
       </c>
       <c r="E131" s="33" t="s">
-        <v>331</v>
+        <v>337</v>
       </c>
       <c r="F131" s="11" t="s">
         <v>112</v>
@@ -7461,7 +7461,7 @@
         <v>491</v>
       </c>
       <c r="E132" s="33" t="s">
-        <v>331</v>
+        <v>337</v>
       </c>
       <c r="F132" s="11" t="s">
         <v>117</v>
@@ -7503,7 +7503,7 @@
         <v>492</v>
       </c>
       <c r="E133" s="33" t="s">
-        <v>331</v>
+        <v>337</v>
       </c>
       <c r="F133" s="11" t="s">
         <v>120</v>
@@ -7545,7 +7545,7 @@
         <v>495</v>
       </c>
       <c r="E134" s="33" t="s">
-        <v>331</v>
+        <v>337</v>
       </c>
       <c r="F134" s="11" t="s">
         <v>121</v>
@@ -7587,7 +7587,7 @@
         <v>496</v>
       </c>
       <c r="E135" s="33" t="s">
-        <v>331</v>
+        <v>337</v>
       </c>
       <c r="F135" s="11" t="s">
         <v>125</v>
@@ -7629,7 +7629,7 @@
         <v>497</v>
       </c>
       <c r="E136" s="33" t="s">
-        <v>331</v>
+        <v>337</v>
       </c>
       <c r="F136" s="11" t="s">
         <v>130</v>
@@ -7670,8 +7670,8 @@
       <c r="D137" s="38" t="s">
         <v>498</v>
       </c>
-      <c r="E137" s="33" t="s">
-        <v>331</v>
+      <c r="E137" s="17" t="s">
+        <v>278</v>
       </c>
       <c r="F137" s="11" t="s">
         <v>133</v>
@@ -7713,7 +7713,7 @@
         <v>140</v>
       </c>
       <c r="E138" s="33" t="s">
-        <v>148</v>
+        <v>458</v>
       </c>
       <c r="G138" s="9"/>
       <c r="H138" s="12"/>
@@ -7752,7 +7752,7 @@
         <v>499</v>
       </c>
       <c r="E139" s="33" t="s">
-        <v>331</v>
+        <v>458</v>
       </c>
       <c r="F139" s="11" t="s">
         <v>152</v>
@@ -7793,8 +7793,8 @@
       <c r="D140" s="39" t="s">
         <v>161</v>
       </c>
-      <c r="E140" s="33" t="s">
-        <v>500</v>
+      <c r="E140" s="17" t="s">
+        <v>10</v>
       </c>
       <c r="F140" s="40"/>
       <c r="G140" s="9"/>
@@ -7834,7 +7834,7 @@
         <v>501</v>
       </c>
       <c r="E141" s="33" t="s">
-        <v>331</v>
+        <v>10</v>
       </c>
       <c r="F141" s="11" t="s">
         <v>165</v>
@@ -7876,7 +7876,7 @@
         <v>502</v>
       </c>
       <c r="E142" s="33" t="s">
-        <v>331</v>
+        <v>271</v>
       </c>
       <c r="F142" s="11" t="s">
         <v>169</v>
@@ -7917,8 +7917,8 @@
       <c r="D143" s="38" t="s">
         <v>503</v>
       </c>
-      <c r="E143" s="33" t="s">
-        <v>331</v>
+      <c r="E143" s="17" t="s">
+        <v>271</v>
       </c>
       <c r="F143" s="11" t="s">
         <v>176</v>
@@ -7960,7 +7960,7 @@
         <v>505</v>
       </c>
       <c r="E144" s="33" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="F144" s="11" t="s">
         <v>506</v>
@@ -8001,8 +8001,8 @@
       <c r="D145" s="38" t="s">
         <v>507</v>
       </c>
-      <c r="E145" s="33" t="s">
-        <v>331</v>
+      <c r="E145" s="17" t="s">
+        <v>107</v>
       </c>
       <c r="F145" s="11" t="s">
         <v>191</v>
@@ -8044,7 +8044,7 @@
         <v>508</v>
       </c>
       <c r="E146" s="33" t="s">
-        <v>331</v>
+        <v>286</v>
       </c>
       <c r="F146" s="11" t="s">
         <v>203</v>
@@ -33393,6 +33393,9 @@
       <c r="AB990" s="12"/>
     </row>
   </sheetData>
+  <sortState ref="E2:E990">
+    <sortCondition ref="E2:E990"/>
+  </sortState>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1"/>
     <hyperlink ref="D3" r:id="rId2"/>

</xml_diff>